<commit_message>
updated assumptions and constraints
</commit_message>
<xml_diff>
--- a/public/assets/assumptions.xlsx
+++ b/public/assets/assumptions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Favour-Daniel\Desktop\Projects\University\ECO\data\processed\inspect\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Favour-Daniel\Desktop\Projects\University\ECO\ECO-Website\public\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{13DFF4C4-E032-4D98-8705-8BC5FBE1B20E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F1EB8D5-9CF4-4F90-867C-DF06E1CD270D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{4AE48245-1A91-4381-8017-F56714F61CFA}"/>
+    <workbookView xWindow="345" yWindow="3045" windowWidth="28530" windowHeight="16245" xr2:uid="{4AE48245-1A91-4381-8017-F56714F61CFA}"/>
   </bookViews>
   <sheets>
     <sheet name="assumptions" sheetId="1" r:id="rId1"/>
@@ -112,9 +112,6 @@
     <t>Raft Material</t>
   </si>
   <si>
-    <t>Steel tile with</t>
-  </si>
-  <si>
     <t>Ceilings Material</t>
   </si>
   <si>
@@ -130,13 +127,16 @@
     <t>OSB topper (Office)</t>
   </si>
   <si>
-    <t>screed</t>
-  </si>
-  <si>
     <t>Floors Material</t>
   </si>
   <si>
     <t>70mm</t>
+  </si>
+  <si>
+    <t>Steel Tile</t>
+  </si>
+  <si>
+    <t>Screed</t>
   </si>
 </sst>
 </file>
@@ -1017,7 +1017,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1315,46 +1315,46 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="1" t="s">
+      <c r="C27" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>36</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>